<commit_message>
change char -> string
</commit_message>
<xml_diff>
--- a/descriptions/abbrevation list.xlsx
+++ b/descriptions/abbrevation list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baseo\git\secad\descriptions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\secad\descriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A544B9-D620-468C-8E1D-430B69142CD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EA96E3-1732-40C8-AC1A-42F41680489A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1694E2A7-7343-4FC2-8908-758DE924B75C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{1694E2A7-7343-4FC2-8908-758DE924B75C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -433,9 +433,6 @@
     <t>wheelhause</t>
   </si>
   <si>
-    <t>char</t>
-  </si>
-  <si>
     <t>Родительский блок по длине</t>
   </si>
   <si>
@@ -824,13 +821,16 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -860,13 +860,6 @@
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
     </font>
     <font>
       <sz val="14"/>
@@ -909,32 +902,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -949,10 +941,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -990,7 +986,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1096,7 +1092,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1249,10 +1245,10 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1262,7 +1258,7 @@
     <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="91.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="72.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1277,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>25</v>
@@ -1285,8 +1281,8 @@
       <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>253</v>
+      <c r="F1" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>107</v>
@@ -1299,7 +1295,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1314,8 +1310,8 @@
       <c r="E2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>254</v>
+      <c r="F2" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>108</v>
@@ -1328,7 +1324,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
+      <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1341,8 +1337,8 @@
       <c r="E3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>254</v>
+      <c r="F3" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>108</v>
@@ -1354,35 +1350,35 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>254</v>
+      <c r="F4" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1395,8 +1391,8 @@
       <c r="E5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>254</v>
+      <c r="F5" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>108</v>
@@ -1409,7 +1405,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1419,8 +1415,8 @@
       <c r="E6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>254</v>
+      <c r="F6" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>108</v>
@@ -1433,7 +1429,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1443,8 +1439,8 @@
       <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>254</v>
+      <c r="F7" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>108</v>
@@ -1457,7 +1453,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1470,8 +1466,8 @@
       <c r="E8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>254</v>
+      <c r="F8" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>108</v>
@@ -1484,12 +1480,12 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>27</v>
@@ -1497,8 +1493,8 @@
       <c r="E9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>254</v>
+      <c r="F9" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>108</v>
@@ -1511,7 +1507,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1524,8 +1520,8 @@
       <c r="E10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>254</v>
+      <c r="F10" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>108</v>
@@ -1538,7 +1534,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1551,8 +1547,8 @@
       <c r="E11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>254</v>
+      <c r="F11" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>108</v>
@@ -1565,7 +1561,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1575,8 +1571,8 @@
       <c r="E12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>254</v>
+      <c r="F12" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>108</v>
@@ -1589,7 +1585,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1599,8 +1595,8 @@
       <c r="E13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>254</v>
+      <c r="F13" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>108</v>
@@ -1613,7 +1609,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
       <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1626,7 +1622,7 @@
       <c r="E14" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>10</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1640,7 +1636,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1650,7 +1646,7 @@
       <c r="E15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>11</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1664,7 +1660,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
       <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1674,7 +1670,7 @@
       <c r="E16" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>12</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1688,7 +1684,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
+      <c r="A17" s="6"/>
       <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1701,7 +1697,7 @@
       <c r="E17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>13</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1715,7 +1711,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
@@ -1728,7 +1724,7 @@
       <c r="E18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>14</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -1742,7 +1738,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
@@ -1755,7 +1751,7 @@
       <c r="E19" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>15</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -1769,7 +1765,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="7"/>
+      <c r="A20" s="6"/>
       <c r="B20" s="1" t="s">
         <v>93</v>
       </c>
@@ -1779,8 +1775,8 @@
       <c r="E20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>254</v>
+      <c r="F20" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>109</v>
@@ -1792,104 +1788,104 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="7"/>
-      <c r="B21" s="3" t="s">
+    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="5">
+      <c r="E21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
         <v>25</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7"/>
-      <c r="B22" s="3" t="s">
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" s="5">
+      <c r="E22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="4">
         <v>26</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="H22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7"/>
-      <c r="B23" s="3" t="s">
+    <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6"/>
+      <c r="B23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" s="5">
+      <c r="E23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="4">
         <v>27</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="H23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="3" t="s">
+    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6"/>
+      <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="5">
+      <c r="E24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
         <v>28</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="7"/>
+      <c r="A25" s="6"/>
       <c r="B25" s="1" t="s">
         <v>77</v>
       </c>
@@ -1899,10 +1895,10 @@
       <c r="D25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" s="5">
+      <c r="E25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
         <v>29</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -1916,17 +1912,17 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="7"/>
+      <c r="A26" s="6"/>
       <c r="B26" s="1" t="s">
         <v>103</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F26" s="5">
+        <v>209</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
         <v>31</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -1936,21 +1932,21 @@
         <v>105</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="7"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" s="5">
+        <v>210</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
         <v>32</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -1960,217 +1956,217 @@
         <v>106</v>
       </c>
       <c r="I27" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="6"/>
+      <c r="B28" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <v>52</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="I28" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="7"/>
-      <c r="B28" s="1" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="6"/>
+      <c r="B29" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5">
-        <v>52</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H28" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="7"/>
-      <c r="B29" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
-        <v>178</v>
+      <c r="A30" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F30" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="F30" s="4" t="s">
+        <v>253</v>
+      </c>
       <c r="G30" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="7"/>
+      <c r="A31" s="6"/>
       <c r="B31" s="1" t="s">
         <v>111</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I31" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>219</v>
-      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
+      <c r="A32" s="6"/>
       <c r="B32" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F32" s="5" t="s">
+      <c r="E32" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="F32" s="4" t="s">
+        <v>253</v>
+      </c>
       <c r="G32" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
+      <c r="A33" s="6"/>
       <c r="B33" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="E33" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="F33" s="4" t="s">
+        <v>253</v>
+      </c>
       <c r="G33" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
+      <c r="A34" s="6"/>
       <c r="B34" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F34" s="5" t="s">
+      <c r="E34" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="F34" s="4" t="s">
+        <v>253</v>
+      </c>
       <c r="G34" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
+      <c r="A35" s="6"/>
       <c r="B35" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="F35" s="5" t="s">
+      <c r="E35" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="F35" s="4" t="s">
+        <v>253</v>
+      </c>
       <c r="G35" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="7"/>
+      <c r="A36" s="6"/>
       <c r="B36" s="1" t="s">
         <v>117</v>
       </c>
@@ -2180,21 +2176,21 @@
       <c r="E36" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>254</v>
+      <c r="F36" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
+      <c r="A37" s="6"/>
       <c r="B37" s="1" t="s">
         <v>118</v>
       </c>
@@ -2204,21 +2200,21 @@
       <c r="E37" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>254</v>
+      <c r="F37" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
+      <c r="A38" s="6"/>
       <c r="B38" s="1" t="s">
         <v>119</v>
       </c>
@@ -2228,21 +2224,21 @@
       <c r="E38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="4" t="s">
-        <v>254</v>
+      <c r="F38" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
+      <c r="A39" s="6"/>
       <c r="B39" s="1" t="s">
         <v>120</v>
       </c>
@@ -2252,21 +2248,21 @@
       <c r="E39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>254</v>
+      <c r="F39" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
+      <c r="A40" s="6"/>
       <c r="B40" s="1" t="s">
         <v>121</v>
       </c>
@@ -2276,21 +2272,21 @@
       <c r="E40" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>254</v>
+      <c r="F40" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
+      <c r="A41" s="6"/>
       <c r="B41" s="1" t="s">
         <v>122</v>
       </c>
@@ -2300,74 +2296,74 @@
       <c r="E41" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F41" s="4" t="s">
-        <v>254</v>
+      <c r="F41" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
+      <c r="A42" s="6"/>
       <c r="B42" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F42" s="4" t="s">
-        <v>254</v>
+      <c r="F42" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>128</v>
+        <v>258</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
+      <c r="A43" s="6"/>
       <c r="B43" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F43" s="4" t="s">
-        <v>254</v>
+      <c r="F43" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G43" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H43" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="H43" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="I43" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="7"/>
+      <c r="A44" s="6"/>
       <c r="B44" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>26</v>
@@ -2375,74 +2371,74 @@
       <c r="E44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F44" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="G44" s="1" t="s">
+      <c r="F44" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>108</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I44" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="6"/>
+      <c r="B45" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I45" s="1" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="7"/>
-      <c r="B45" s="1" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="6"/>
+      <c r="B46" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="I45" s="1" t="s">
+      <c r="E46" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
-      <c r="B46" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I46" s="1" t="s">
-        <v>235</v>
-      </c>
-    </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="7"/>
+      <c r="A47" s="6"/>
       <c r="B47" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>26</v>
@@ -2450,26 +2446,26 @@
       <c r="E47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F47" s="4">
+      <c r="F47" s="3">
         <v>16</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H47" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="6"/>
+      <c r="B48" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="I47" s="1" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="B48" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="C48" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>26</v>
@@ -2477,26 +2473,26 @@
       <c r="E48" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F48" s="3">
         <v>17</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H48" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="6"/>
+      <c r="B49" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
-      <c r="B49" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>26</v>
@@ -2504,107 +2500,107 @@
       <c r="E49" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F49" s="4">
+      <c r="F49" s="3">
         <v>18</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H49" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="6"/>
+      <c r="B50" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="I49" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <v>19</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I50" s="1" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="7"/>
-      <c r="B50" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D50" s="1" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="6"/>
+      <c r="B51" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F50" s="4">
-        <v>19</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="7"/>
-      <c r="B51" s="1" t="s">
+      <c r="E51" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3">
+        <v>20</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="6"/>
+      <c r="B52" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F51" s="4">
-        <v>20</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H51" s="1" t="s">
+      <c r="D52" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3">
+        <v>21</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H52" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="7"/>
-      <c r="B52" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F52" s="4">
-        <v>21</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H52" s="1" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="6"/>
+      <c r="B53" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I52" s="1" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="7"/>
-      <c r="B53" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="C53" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>26</v>
@@ -2612,26 +2608,26 @@
       <c r="E53" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F53" s="4">
+      <c r="F53" s="3">
         <v>22</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="7"/>
+      <c r="A54" s="6"/>
       <c r="B54" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>26</v>
@@ -2639,247 +2635,247 @@
       <c r="E54" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F54" s="4">
+      <c r="F54" s="3">
         <v>23</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="7"/>
+      <c r="A55" s="6"/>
       <c r="B55" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>256</v>
+      <c r="E55" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>255</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="7"/>
+      <c r="A56" s="6"/>
       <c r="B56" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>256</v>
+      <c r="E56" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>255</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="8" t="s">
-        <v>185</v>
+      <c r="A57" s="7" t="s">
+        <v>184</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F57" s="4" t="s">
-        <v>254</v>
+      <c r="F57" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="8"/>
+      <c r="A58" s="7"/>
       <c r="B58" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F58" s="4" t="s">
-        <v>254</v>
+      <c r="F58" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="8"/>
+      <c r="A59" s="7"/>
       <c r="B59" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F59" s="4" t="s">
-        <v>254</v>
+      <c r="F59" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I59" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A60" s="7"/>
+      <c r="B60" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="I60" s="1" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="8"/>
-      <c r="B60" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F60" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="G60" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H60" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I60" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
     <row r="61" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="9" t="s">
-        <v>187</v>
+      <c r="A61" s="8" t="s">
+        <v>186</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F61" s="4" t="s">
-        <v>254</v>
+      <c r="F61" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="9"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>254</v>
+      <c r="F62" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>109</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="9"/>
+      <c r="A63" s="8"/>
       <c r="B63" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>254</v>
+      <c r="F63" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="6"/>
+      <c r="A64" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Block's integers are described
</commit_message>
<xml_diff>
--- a/descriptions/abbrevation list.xlsx
+++ b/descriptions/abbrevation list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\secad\descriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EA96E3-1732-40C8-AC1A-42F41680489A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A21ACA1-F6D0-4B9C-82F5-6EEFDC7D1A77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{1694E2A7-7343-4FC2-8908-758DE924B75C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="271">
   <si>
     <t>Расчёт</t>
   </si>
@@ -430,9 +430,6 @@
     <t>funnel</t>
   </si>
   <si>
-    <t>wheelhause</t>
-  </si>
-  <si>
     <t>Родительский блок по длине</t>
   </si>
   <si>
@@ -574,12 +571,6 @@
     <t>z_g</t>
   </si>
   <si>
-    <t>Абсцисса центра тяжести площади проекции блока на ДП</t>
-  </si>
-  <si>
-    <t>Аппликата центра тяжести площади проекции блока на ДП</t>
-  </si>
-  <si>
     <t>Переменные класса блоков</t>
   </si>
   <si>
@@ -745,9 +736,6 @@
     <t>Head block by Length</t>
   </si>
   <si>
-    <t>Length to Head Block by Length</t>
-  </si>
-  <si>
     <t>Slave Block by Height</t>
   </si>
   <si>
@@ -760,18 +748,6 @@
     <t>bb_u</t>
   </si>
   <si>
-    <t>Lower Base Statical Moment</t>
-  </si>
-  <si>
-    <t>Upper Base Statical Moment</t>
-  </si>
-  <si>
-    <t>Block's Gravity Center Ordinate</t>
-  </si>
-  <si>
-    <t>Block's Gravity Center Applicate</t>
-  </si>
-  <si>
     <t>Block's Fore Upper Point</t>
   </si>
   <si>
@@ -824,6 +800,66 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>blocktitle</t>
+  </si>
+  <si>
+    <t>Block Title</t>
+  </si>
+  <si>
+    <t>Название блока</t>
+  </si>
+  <si>
+    <t>cont</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>Название класса</t>
+  </si>
+  <si>
+    <t>Optimized Continious Class</t>
+  </si>
+  <si>
+    <t>Optimized Descrete Class</t>
+  </si>
+  <si>
+    <t>Постоянная переменная</t>
+  </si>
+  <si>
+    <t>cons</t>
+  </si>
+  <si>
+    <t>Constant Integer</t>
+  </si>
+  <si>
+    <t>wheelhouse</t>
+  </si>
+  <si>
+    <t>Distance to Head Block by Length</t>
+  </si>
+  <si>
+    <t>Block's Lower Base Statical Moment</t>
+  </si>
+  <si>
+    <t>Block's Upper Base Statical Moment</t>
+  </si>
+  <si>
+    <t>Block's Proection Area to CL Gravity Center (CG) Ordinate</t>
+  </si>
+  <si>
+    <t>Block's Proection Area to CL CG Applicate</t>
+  </si>
+  <si>
+    <t>Абсцисса центра тяжести (ЦТ) площади проекции блока на ДП</t>
+  </si>
+  <si>
+    <t>Аппликата ЦТ площади проекции блока на ДП</t>
   </si>
 </sst>
 </file>
@@ -939,10 +975,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1242,13 +1274,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B698AE2B-A9EB-4E3F-AD61-60D9D0032DF1}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1270,10 +1302,10 @@
         <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>251</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>25</v>
@@ -1282,7 +1314,7 @@
         <v>30</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>107</v>
@@ -1311,7 +1343,7 @@
         <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>108</v>
@@ -1338,7 +1370,7 @@
         <v>31</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>108</v>
@@ -1365,7 +1397,7 @@
         <v>31</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>108</v>
@@ -1392,7 +1424,7 @@
         <v>31</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>108</v>
@@ -1416,7 +1448,7 @@
         <v>31</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>108</v>
@@ -1440,7 +1472,7 @@
         <v>31</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>108</v>
@@ -1467,7 +1499,7 @@
         <v>31</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>108</v>
@@ -1485,7 +1517,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>27</v>
@@ -1494,7 +1526,7 @@
         <v>31</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>108</v>
@@ -1521,7 +1553,7 @@
         <v>31</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>108</v>
@@ -1548,7 +1580,7 @@
         <v>31</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>108</v>
@@ -1572,7 +1604,7 @@
         <v>31</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>108</v>
@@ -1596,7 +1628,7 @@
         <v>31</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>108</v>
@@ -1776,7 +1808,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>109</v>
@@ -1917,7 +1949,7 @@
         <v>103</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>0</v>
@@ -1932,7 +1964,7 @@
         <v>105</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1941,7 +1973,7 @@
         <v>104</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>0</v>
@@ -1956,16 +1988,16 @@
         <v>106</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
       <c r="B28" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>0</v>
@@ -1977,495 +2009,492 @@
         <v>108</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
       <c r="B29" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>110</v>
+        <v>245</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>216</v>
+        <v>252</v>
       </c>
       <c r="E30" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="H30" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="I30" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="G30" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="6"/>
       <c r="B32" s="1" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>28</v>
+        <v>214</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
       <c r="B33" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="6"/>
       <c r="B34" s="1" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>150</v>
+        <v>219</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
       <c r="B35" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>26</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="B36" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>253</v>
+        <v>150</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>245</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
       <c r="B37" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>115</v>
+        <v>222</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
       <c r="B38" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>226</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
       <c r="B39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
       <c r="B40" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
       <c r="B41" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G41" s="1" t="s">
         <v>116</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
       <c r="B42" s="1" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>132</v>
+        <v>263</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>258</v>
+        <v>245</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="B43" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>128</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
       <c r="B44" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>26</v>
+        <v>132</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>108</v>
+        <v>250</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
       <c r="B45" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>134</v>
+        <v>140</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>258</v>
+        <v>108</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>233</v>
+        <v>264</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
       <c r="B46" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>130</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="1" t="s">
-        <v>44</v>
+        <v>138</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F47" s="3">
-        <v>16</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>108</v>
+      <c r="F47" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="1" t="s">
-        <v>160</v>
+        <v>44</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>26</v>
@@ -2474,25 +2503,25 @@
         <v>0</v>
       </c>
       <c r="F48" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>162</v>
+        <v>232</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>26</v>
@@ -2501,133 +2530,133 @@
         <v>0</v>
       </c>
       <c r="F49" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>178</v>
+        <v>26</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F50" s="3">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F51" s="3">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F52" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>238</v>
+        <v>265</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="1" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>26</v>
+        <v>176</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F53" s="3">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>239</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>26</v>
@@ -2636,52 +2665,52 @@
         <v>0</v>
       </c>
       <c r="F54" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>176</v>
+        <v>269</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>240</v>
+        <v>267</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="1" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>202</v>
+        <v>173</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="E55" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>255</v>
+      <c r="F55" s="3">
+        <v>23</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>191</v>
+        <v>270</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>26</v>
@@ -2690,199 +2719,297 @@
         <v>0</v>
       </c>
       <c r="F56" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A57" s="6"/>
+      <c r="B57" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="G56" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="I56" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="E57" s="1" t="s">
+      <c r="E58" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="7"/>
-      <c r="B58" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>108</v>
+      <c r="F58" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>193</v>
+        <v>257</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7"/>
       <c r="B59" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="7"/>
       <c r="B60" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="8" t="s">
-        <v>186</v>
-      </c>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A61" s="7"/>
       <c r="B61" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="8"/>
+      <c r="A62" s="7"/>
       <c r="B62" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E62" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A63" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G62" s="1" t="s">
+      <c r="F63" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="8"/>
+      <c r="B64" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="8"/>
+      <c r="B65" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G65" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="H62" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="I62" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="8"/>
-      <c r="B63" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="E63" s="1" t="s">
+      <c r="H65" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="8"/>
+      <c r="B66" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F63" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="I63" s="1" t="s">
+      <c r="F66" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I66" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="A67" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="5"/>
+      <c r="H67" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="I67" s="1" t="s">
+        <v>262</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="A63:A66"/>
     <mergeCell ref="A2:A29"/>
-    <mergeCell ref="A30:A56"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A30:A57"/>
+    <mergeCell ref="A58:A62"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rename desc -> disc
</commit_message>
<xml_diff>
--- a/descriptions/abbrevation list.xlsx
+++ b/descriptions/abbrevation list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\secad\descriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A21ACA1-F6D0-4B9C-82F5-6EEFDC7D1A77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D6C15E-9AF2-43B0-B4A6-B16CF42D7E2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{1694E2A7-7343-4FC2-8908-758DE924B75C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1694E2A7-7343-4FC2-8908-758DE924B75C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -817,18 +817,12 @@
     <t>cont</t>
   </si>
   <si>
-    <t>desc</t>
-  </si>
-  <si>
     <t>Название класса</t>
   </si>
   <si>
     <t>Optimized Continious Class</t>
   </si>
   <si>
-    <t>Optimized Descrete Class</t>
-  </si>
-  <si>
     <t>Постоянная переменная</t>
   </si>
   <si>
@@ -860,6 +854,12 @@
   </si>
   <si>
     <t>Аппликата ЦТ площади проекции блока на ДП</t>
+  </si>
+  <si>
+    <t>disc</t>
+  </si>
+  <si>
+    <t>Optimized Discrete Class</t>
   </si>
 </sst>
 </file>
@@ -951,13 +951,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1277,10 +1277,10 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
+      <selection pane="bottomRight" activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1327,7 +1327,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1356,7 +1356,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1383,7 +1383,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1410,7 +1410,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1437,7 +1437,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1539,7 +1539,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1566,7 +1566,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1593,7 +1593,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1617,7 +1617,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1641,7 +1641,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1668,7 +1668,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1692,7 +1692,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1716,7 +1716,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
       <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
@@ -1743,7 +1743,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
@@ -1770,7 +1770,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
+      <c r="A19" s="7"/>
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
@@ -1797,7 +1797,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>93</v>
       </c>
@@ -1821,7 +1821,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
         <v>49</v>
       </c>
@@ -1845,7 +1845,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
@@ -1869,7 +1869,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="2" t="s">
         <v>51</v>
       </c>
@@ -1893,7 +1893,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
@@ -1917,7 +1917,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="1" t="s">
         <v>77</v>
       </c>
@@ -1944,7 +1944,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="1" t="s">
         <v>103</v>
       </c>
@@ -1968,7 +1968,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="1" t="s">
         <v>104</v>
       </c>
@@ -1992,7 +1992,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="1" t="s">
         <v>184</v>
       </c>
@@ -2016,7 +2016,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="1" t="s">
         <v>185</v>
       </c>
@@ -2040,7 +2040,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="7" t="s">
         <v>174</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="1" t="s">
         <v>110</v>
       </c>
@@ -2090,7 +2090,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="1" t="s">
         <v>111</v>
       </c>
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="1" t="s">
         <v>145</v>
       </c>
@@ -2141,7 +2141,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="1" t="s">
         <v>146</v>
       </c>
@@ -2168,7 +2168,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="1" t="s">
         <v>112</v>
       </c>
@@ -2195,7 +2195,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="1" t="s">
         <v>113</v>
       </c>
@@ -2222,7 +2222,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="1" t="s">
         <v>117</v>
       </c>
@@ -2246,7 +2246,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="1" t="s">
         <v>118</v>
       </c>
@@ -2270,7 +2270,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="6"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="1" t="s">
         <v>119</v>
       </c>
@@ -2294,7 +2294,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="6"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="1" t="s">
         <v>120</v>
       </c>
@@ -2318,7 +2318,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="1" t="s">
         <v>121</v>
       </c>
@@ -2342,12 +2342,12 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>31</v>
@@ -2366,7 +2366,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
+      <c r="A43" s="7"/>
       <c r="B43" s="1" t="s">
         <v>135</v>
       </c>
@@ -2390,7 +2390,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="6"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="1" t="s">
         <v>136</v>
       </c>
@@ -2414,7 +2414,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="6"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="1" t="s">
         <v>139</v>
       </c>
@@ -2437,11 +2437,11 @@
         <v>157</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="6"/>
+      <c r="A46" s="7"/>
       <c r="B46" s="1" t="s">
         <v>137</v>
       </c>
@@ -2465,7 +2465,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="6"/>
+      <c r="A47" s="7"/>
       <c r="B47" s="1" t="s">
         <v>138</v>
       </c>
@@ -2489,7 +2489,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="6"/>
+      <c r="A48" s="7"/>
       <c r="B48" s="1" t="s">
         <v>44</v>
       </c>
@@ -2516,7 +2516,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="6"/>
+      <c r="A49" s="7"/>
       <c r="B49" s="1" t="s">
         <v>159</v>
       </c>
@@ -2543,7 +2543,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="6"/>
+      <c r="A50" s="7"/>
       <c r="B50" s="1" t="s">
         <v>161</v>
       </c>
@@ -2570,7 +2570,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="6"/>
+      <c r="A51" s="7"/>
       <c r="B51" s="1" t="s">
         <v>163</v>
       </c>
@@ -2597,7 +2597,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="6"/>
+      <c r="A52" s="7"/>
       <c r="B52" s="1" t="s">
         <v>166</v>
       </c>
@@ -2620,11 +2620,11 @@
         <v>170</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="6"/>
+      <c r="A53" s="7"/>
       <c r="B53" s="1" t="s">
         <v>167</v>
       </c>
@@ -2647,11 +2647,11 @@
         <v>171</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="6"/>
+      <c r="A54" s="7"/>
       <c r="B54" s="1" t="s">
         <v>172</v>
       </c>
@@ -2671,14 +2671,14 @@
         <v>108</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="6"/>
+      <c r="A55" s="7"/>
       <c r="B55" s="1" t="s">
         <v>173</v>
       </c>
@@ -2698,14 +2698,14 @@
         <v>108</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="6"/>
+      <c r="A56" s="7"/>
       <c r="B56" s="1" t="s">
         <v>186</v>
       </c>
@@ -2732,7 +2732,7 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="6"/>
+      <c r="A57" s="7"/>
       <c r="B57" s="1" t="s">
         <v>187</v>
       </c>
@@ -2759,7 +2759,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="8" t="s">
         <v>181</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2778,14 +2778,14 @@
         <v>250</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="I58" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="I58" s="1" t="s">
-        <v>258</v>
-      </c>
     </row>
     <row r="59" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="7"/>
+      <c r="A59" s="8"/>
       <c r="B59" s="1" t="s">
         <v>177</v>
       </c>
@@ -2809,7 +2809,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="7"/>
+      <c r="A60" s="8"/>
       <c r="B60" s="1" t="s">
         <v>178</v>
       </c>
@@ -2833,7 +2833,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="7"/>
+      <c r="A61" s="8"/>
       <c r="B61" s="1" t="s">
         <v>179</v>
       </c>
@@ -2857,7 +2857,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="7"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="1" t="s">
         <v>180</v>
       </c>
@@ -2881,14 +2881,14 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="6" t="s">
         <v>183</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>256</v>
+        <v>269</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>31</v>
@@ -2900,14 +2900,14 @@
         <v>250</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="8"/>
+      <c r="A64" s="6"/>
       <c r="B64" s="1" t="s">
         <v>177</v>
       </c>
@@ -2931,7 +2931,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="8"/>
+      <c r="A65" s="6"/>
       <c r="B65" s="1" t="s">
         <v>182</v>
       </c>
@@ -2955,7 +2955,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="8"/>
+      <c r="A66" s="6"/>
       <c r="B66" s="1" t="s">
         <v>180</v>
       </c>
@@ -2980,13 +2980,13 @@
     </row>
     <row r="67" spans="1:9" ht="28.5" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>245</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>31</v>
@@ -2998,10 +2998,10 @@
         <v>250</v>
       </c>
       <c r="H67" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="I67" s="1" t="s">
         <v>260</v>
-      </c>
-      <c r="I67" s="1" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
description.docx: block's applicate determination is added + unimportant fix
</commit_message>
<xml_diff>
--- a/descriptions/abbrevation list.xlsx
+++ b/descriptions/abbrevation list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\secad\descriptions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\secad\descriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D6C15E-9AF2-43B0-B4A6-B16CF42D7E2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62B1C3D-762A-4161-95B0-621EC5F89B5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1694E2A7-7343-4FC2-8908-758DE924B75C}"/>
   </bookViews>
@@ -1277,10 +1277,10 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I63" sqref="I63"/>
+      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2206,7 +2206,7 @@
         <v>26</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>245</v>

</xml_diff>

<commit_message>
change red color to black. I hate red
</commit_message>
<xml_diff>
--- a/descriptions/abbrevation list.xlsx
+++ b/descriptions/abbrevation list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\secad\descriptions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\baseo\git\secad\descriptions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36ED388-D391-4318-A98A-C918690D4ED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A87431B-8B2E-4DE4-94C5-744E2133CBA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{1694E2A7-7343-4FC2-8908-758DE924B75C}"/>
+    <workbookView xWindow="5730" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{1694E2A7-7343-4FC2-8908-758DE924B75C}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="270">
   <si>
     <t>Расчёт</t>
   </si>
@@ -863,7 +863,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -914,13 +914,6 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -955,10 +948,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -968,9 +957,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -986,9 +981,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1026,7 +1021,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1132,7 +1127,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1285,10 +1280,10 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B21" sqref="A21:XFD24"/>
+      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1335,7 +1330,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1364,7 +1359,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1391,7 +1386,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1418,7 +1413,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1445,7 +1440,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="9"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1469,7 +1464,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1493,7 +1488,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1520,7 +1515,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="20.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1547,7 +1542,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1574,7 +1569,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1601,7 +1596,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1625,7 +1620,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1649,7 +1644,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
+      <c r="A14" s="7"/>
       <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
@@ -1676,7 +1671,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+      <c r="A15" s="7"/>
       <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
@@ -1700,7 +1695,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+      <c r="A16" s="7"/>
       <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
@@ -1723,35 +1718,35 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9"/>
-      <c r="B17" s="6" t="s">
+    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7"/>
+      <c r="B17" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="4">
         <v>13</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="G17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="9"/>
+      <c r="A18" s="7"/>
       <c r="B18" s="1" t="s">
         <v>40</v>
       </c>
@@ -1777,35 +1772,35 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="4">
         <v>15</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H19" s="6" t="s">
+      <c r="G19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="9"/>
+      <c r="A20" s="7"/>
       <c r="B20" s="1" t="s">
         <v>93</v>
       </c>
@@ -1828,104 +1823,104 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9"/>
-      <c r="B21" s="6" t="s">
+    <row r="21" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="4">
         <v>28</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H21" s="6" t="s">
+      <c r="G21" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9"/>
-      <c r="B22" s="6" t="s">
+    <row r="22" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="4">
         <v>29</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22" s="6" t="s">
+      <c r="G22" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I22" s="6" t="s">
+      <c r="I22" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7"/>
+      <c r="B23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="4">
         <v>30</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H23" s="6" t="s">
+      <c r="G23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="6" t="s">
+    <row r="24" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7"/>
+      <c r="B24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="4">
         <v>31</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H24" s="6" t="s">
+      <c r="G24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="6" t="s">
+      <c r="I24" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="1" t="s">
         <v>77</v>
       </c>
@@ -1952,7 +1947,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="1" t="s">
         <v>103</v>
       </c>
@@ -1976,7 +1971,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="1" t="s">
         <v>104</v>
       </c>
@@ -2000,7 +1995,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="1" t="s">
         <v>184</v>
       </c>
@@ -2024,7 +2019,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="1" t="s">
         <v>185</v>
       </c>
@@ -2048,7 +2043,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="7" t="s">
         <v>174</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -2074,7 +2069,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="1" t="s">
         <v>110</v>
       </c>
@@ -2098,7 +2093,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="1" t="s">
         <v>111</v>
       </c>
@@ -2122,7 +2117,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="1" t="s">
         <v>145</v>
       </c>
@@ -2149,7 +2144,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="1" t="s">
         <v>146</v>
       </c>
@@ -2176,7 +2171,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="9"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="1" t="s">
         <v>112</v>
       </c>
@@ -2203,7 +2198,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="1" t="s">
         <v>113</v>
       </c>
@@ -2216,8 +2211,8 @@
       <c r="E36" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>243</v>
+      <c r="F36" s="4">
+        <v>16</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>108</v>
@@ -2230,7 +2225,7 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="1" t="s">
         <v>117</v>
       </c>
@@ -2254,7 +2249,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="1" t="s">
         <v>118</v>
       </c>
@@ -2278,7 +2273,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="1" t="s">
         <v>119</v>
       </c>
@@ -2302,7 +2297,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="1" t="s">
         <v>120</v>
       </c>
@@ -2326,7 +2321,7 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="1" t="s">
         <v>121</v>
       </c>
@@ -2350,7 +2345,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="1" t="s">
         <v>122</v>
       </c>
@@ -2374,7 +2369,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
+      <c r="A43" s="7"/>
       <c r="B43" s="1" t="s">
         <v>135</v>
       </c>
@@ -2398,7 +2393,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="1" t="s">
         <v>136</v>
       </c>
@@ -2422,7 +2417,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="9"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="1" t="s">
         <v>139</v>
       </c>
@@ -2449,7 +2444,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
+      <c r="A46" s="7"/>
       <c r="B46" s="1" t="s">
         <v>137</v>
       </c>
@@ -2473,7 +2468,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="9"/>
+      <c r="A47" s="7"/>
       <c r="B47" s="1" t="s">
         <v>138</v>
       </c>
@@ -2497,7 +2492,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="9"/>
+      <c r="A48" s="7"/>
       <c r="B48" s="1" t="s">
         <v>44</v>
       </c>
@@ -2511,7 +2506,7 @@
         <v>0</v>
       </c>
       <c r="F48" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>108</v>
@@ -2524,7 +2519,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
+      <c r="A49" s="7"/>
       <c r="B49" s="1" t="s">
         <v>159</v>
       </c>
@@ -2538,7 +2533,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>108</v>
@@ -2551,7 +2546,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="9"/>
+      <c r="A50" s="7"/>
       <c r="B50" s="1" t="s">
         <v>161</v>
       </c>
@@ -2565,7 +2560,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="3">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>108</v>
@@ -2578,7 +2573,7 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
+      <c r="A51" s="7"/>
       <c r="B51" s="1" t="s">
         <v>163</v>
       </c>
@@ -2592,7 +2587,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>108</v>
@@ -2605,7 +2600,7 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
+      <c r="A52" s="7"/>
       <c r="B52" s="1" t="s">
         <v>166</v>
       </c>
@@ -2619,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>108</v>
@@ -2632,7 +2627,7 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
+      <c r="A53" s="7"/>
       <c r="B53" s="1" t="s">
         <v>167</v>
       </c>
@@ -2645,8 +2640,8 @@
       <c r="E53" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F53" s="3">
-        <v>21</v>
+      <c r="F53" s="9">
+        <v>22</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>108</v>
@@ -2658,35 +2653,35 @@
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="9"/>
-      <c r="B54" s="6" t="s">
+    <row r="54" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="7"/>
+      <c r="B54" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="6" t="s">
+      <c r="E54" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F54" s="7">
-        <v>22</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H54" s="6" t="s">
+      <c r="F54" s="9">
+        <v>23</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H54" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="I54" s="6" t="s">
+      <c r="I54" s="2" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="9"/>
+      <c r="A55" s="7"/>
       <c r="B55" s="1" t="s">
         <v>173</v>
       </c>
@@ -2699,8 +2694,8 @@
       <c r="E55" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F55" s="3">
-        <v>23</v>
+      <c r="F55" s="10">
+        <v>24</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>108</v>
@@ -2712,62 +2707,62 @@
         <v>263</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="9"/>
-      <c r="B56" s="6" t="s">
+    <row r="56" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="7"/>
+      <c r="B56" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="E56" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F56" s="7">
+      <c r="F56" s="4">
         <v>25</v>
       </c>
-      <c r="G56" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H56" s="6" t="s">
+      <c r="G56" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H56" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="I56" s="6" t="s">
+      <c r="I56" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9"/>
-      <c r="B57" s="6" t="s">
+    <row r="57" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7"/>
+      <c r="B57" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E57" s="6" t="s">
+      <c r="E57" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F57" s="7">
+      <c r="F57" s="4">
         <v>26</v>
       </c>
-      <c r="G57" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H57" s="6" t="s">
+      <c r="G57" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="H57" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="I57" s="6" t="s">
+      <c r="I57" s="2" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="8" t="s">
         <v>181</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -2793,7 +2788,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="10"/>
+      <c r="A59" s="8"/>
       <c r="B59" s="1" t="s">
         <v>177</v>
       </c>
@@ -2817,7 +2812,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="10"/>
+      <c r="A60" s="8"/>
       <c r="B60" s="1" t="s">
         <v>178</v>
       </c>
@@ -2841,7 +2836,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="10"/>
+      <c r="A61" s="8"/>
       <c r="B61" s="1" t="s">
         <v>179</v>
       </c>
@@ -2865,7 +2860,7 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="10"/>
+      <c r="A62" s="8"/>
       <c r="B62" s="1" t="s">
         <v>180</v>
       </c>
@@ -2889,7 +2884,7 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="8" t="s">
+      <c r="A63" s="6" t="s">
         <v>183</v>
       </c>
       <c r="B63" s="1" t="s">
@@ -2915,7 +2910,7 @@
       </c>
     </row>
     <row r="64" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="8"/>
+      <c r="A64" s="6"/>
       <c r="B64" s="1" t="s">
         <v>177</v>
       </c>
@@ -2939,7 +2934,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="8"/>
+      <c r="A65" s="6"/>
       <c r="B65" s="1" t="s">
         <v>182</v>
       </c>
@@ -2963,7 +2958,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="8"/>
+      <c r="A66" s="6"/>
       <c r="B66" s="1" t="s">
         <v>180</v>
       </c>

</xml_diff>